<commit_message>
Cada gráfico es una función distinta. Se modifica el orden en que aprecen los gráficos en la hoja Dashboard.
</commit_message>
<xml_diff>
--- a/data/sqm.xlsx
+++ b/data/sqm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alvarodiaz/my_repos/impacto-economico/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09F27C36-16A0-6B49-A157-F746FCFAC049}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27A4E1D1-2A83-014A-A10B-B474868CA3B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19860" activeTab="5" xr2:uid="{69EDB390-A534-AC45-921F-B42152D86256}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19860" activeTab="6" xr2:uid="{69EDB390-A534-AC45-921F-B42152D86256}"/>
   </bookViews>
   <sheets>
     <sheet name="PAIS" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="50">
   <si>
     <t>Pagos</t>
   </si>
@@ -186,6 +186,12 @@
   </si>
   <si>
     <t>Agno</t>
+  </si>
+  <si>
+    <t>Año 2022</t>
+  </si>
+  <si>
+    <t>Año 2023</t>
   </si>
 </sst>
 </file>
@@ -575,7 +581,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -588,10 +594,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -1299,7 +1305,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7076BBED-0D9B-E44C-877A-B2D32BCACD5C}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1439,11 +1445,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59C4B5DF-D502-EF4A-989C-FC461695A943}">
   <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">

</xml_diff>